<commit_message>
updated children task and schedules
</commit_message>
<xml_diff>
--- a/conditions/inputTrain_1.1.xlsx
+++ b/conditions/inputTrain_1.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\45040\Desktop\MCNB\Career\MPI\psychopy_task_trythis\conditions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\45040\gcasa\g-casa_children_task\conditions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF891B9E-C1E7-45FB-B863-651C5BF2C62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F441A11E-8918-46CE-84D4-2736AD9A7EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
   <si>
     <t>trialTrain</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,7 +471,7 @@
         <v>62</v>
       </c>
       <c r="I2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
@@ -503,7 +503,7 @@
         <v>64</v>
       </c>
       <c r="I3">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
         <v>10</v>
@@ -535,7 +535,7 @@
         <v>66</v>
       </c>
       <c r="I4">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -567,7 +567,7 @@
         <v>65</v>
       </c>
       <c r="I5">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -578,28 +578,28 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J6" t="s">
         <v>10</v>
@@ -610,28 +610,28 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I7">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
@@ -642,28 +642,28 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I8">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s">
         <v>10</v>
@@ -674,13 +674,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -689,13 +689,13 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I9">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J9" t="s">
         <v>10</v>
@@ -706,28 +706,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I10">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
         <v>10</v>
@@ -738,28 +738,28 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I11">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
@@ -770,28 +770,28 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J12" t="s">
         <v>10</v>
@@ -802,28 +802,28 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J13" t="s">
         <v>10</v>
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -849,13 +849,13 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I14">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J14" t="s">
         <v>10</v>
@@ -866,28 +866,28 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J15" t="s">
         <v>10</v>
@@ -898,28 +898,28 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I16">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J16" t="s">
         <v>10</v>
@@ -933,25 +933,25 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J17" t="s">
         <v>10</v>
@@ -962,13 +962,13 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <v>7</v>
@@ -977,13 +977,13 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H18">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I18">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J18" t="s">
         <v>10</v>
@@ -997,25 +997,25 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I19">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J19" t="s">
         <v>10</v>
@@ -1026,16 +1026,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1047,7 +1047,7 @@
         <v>62</v>
       </c>
       <c r="I20">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
         <v>10</v>
@@ -1058,16 +1058,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>64</v>
       </c>
       <c r="I21">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J21" t="s">
         <v>10</v>
@@ -1090,28 +1090,28 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I22">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J22" t="s">
         <v>10</v>
@@ -1122,28 +1122,28 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I23">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J23" t="s">
         <v>10</v>
@@ -1154,28 +1154,28 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I24">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J24" t="s">
         <v>10</v>
@@ -1186,30 +1186,222 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>64</v>
+      </c>
+      <c r="I25">
+        <v>30</v>
+      </c>
+      <c r="J25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
         <v>6</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
-      <c r="H25">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>65</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+      <c r="J26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>62</v>
+      </c>
+      <c r="I27">
+        <v>30</v>
+      </c>
+      <c r="J27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>65</v>
+      </c>
+      <c r="I28">
+        <v>30</v>
+      </c>
+      <c r="J28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>61</v>
+      </c>
+      <c r="I29">
+        <v>30</v>
+      </c>
+      <c r="J29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
         <v>66</v>
       </c>
-      <c r="I25">
-        <v>24</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I30">
+        <v>30</v>
+      </c>
+      <c r="J30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>64</v>
+      </c>
+      <c r="I31">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>